<commit_message>
Add code for saving data from dataset to excel file. did not finished yet.
</commit_message>
<xml_diff>
--- a/ImportExcelToDB/xls/西伍商业决策分析系统_功能框架列表.xlsx
+++ b/ImportExcelToDB/xls/西伍商业决策分析系统_功能框架列表.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="系统用户权限分类" sheetId="4" r:id="rId1"/>
     <sheet name="系统功能框架分类" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="173">
   <si>
     <t>功能模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -343,6 +344,282 @@
   <si>
     <t>错误明细提示</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>biid</t>
+  </si>
+  <si>
+    <t>buty</t>
+  </si>
+  <si>
+    <t>dety</t>
+  </si>
+  <si>
+    <t>aity</t>
+  </si>
+  <si>
+    <t>aico</t>
+  </si>
+  <si>
+    <t>soty</t>
+  </si>
+  <si>
+    <t>soco</t>
+  </si>
+  <si>
+    <t>infl</t>
+  </si>
+  <si>
+    <t>flag</t>
+  </si>
+  <si>
+    <t>crus</t>
+  </si>
+  <si>
+    <t>crna</t>
+  </si>
+  <si>
+    <t>crdt</t>
+  </si>
+  <si>
+    <t>edus</t>
+  </si>
+  <si>
+    <t>edna</t>
+  </si>
+  <si>
+    <t>eddt</t>
+  </si>
+  <si>
+    <t>chus</t>
+  </si>
+  <si>
+    <t>chna</t>
+  </si>
+  <si>
+    <t>chdt</t>
+  </si>
+  <si>
+    <t>opna</t>
+  </si>
+  <si>
+    <t>psdt</t>
+  </si>
+  <si>
+    <t>pmmt</t>
+  </si>
+  <si>
+    <t>rsmt</t>
+  </si>
+  <si>
+    <t>whid</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>orid</t>
+  </si>
+  <si>
+    <t>stat</t>
+  </si>
+  <si>
+    <t>rema</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>CP14071300003</t>
+  </si>
+  <si>
+    <t>stockplan</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>STOCKOPT</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>许源贵</t>
+  </si>
+  <si>
+    <t>2014/7/13 13:46:09</t>
+  </si>
+  <si>
+    <t>2014/7/13 14:08:18</t>
+  </si>
+  <si>
+    <t>2014/7/13 0:00:00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>T5-J04-06-04,T5-J04-06-03,T5-J04-06-02,T5-J04-06-01,T5-J03-06-04,T5-J03-06-03,T5-J03-06-02,T5-J03-06-01,T5-J02-06-04,T5-J02-06-03,T5-J02-06-02,T5-J02-06-01,T5-J01-06-04,T5-J01-06-03,T5-J01-06-02,T5-J01-06-01</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>CP14071300004</t>
+  </si>
+  <si>
+    <t>2014/7/13 21:02:58</t>
+  </si>
+  <si>
+    <t>2014/7/13 21:04:22</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>T5-J01-03-06</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>CP14071300005</t>
+  </si>
+  <si>
+    <t>2014/7/13 21:05:01</t>
+  </si>
+  <si>
+    <t>甘天红</t>
+  </si>
+  <si>
+    <t>2014/7/14 14:21:10</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>CP14071400001</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>管理员</t>
+  </si>
+  <si>
+    <t>2014/7/14 14:39:06</t>
+  </si>
+  <si>
+    <t>2014/7/14 14:45:35</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>2014/7/14 0:00:00</t>
+  </si>
+  <si>
+    <t>T1-E06-01-06</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>CP14071400002</t>
+  </si>
+  <si>
+    <t>2014/7/14 19:31:58</t>
+  </si>
+  <si>
+    <t>2014/7/14 19:36:51</t>
+  </si>
+  <si>
+    <t>T1-D09-01-03</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>CP14071500001</t>
+  </si>
+  <si>
+    <t>2014/7/15 8:08:23</t>
+  </si>
+  <si>
+    <t>2014/7/15 8:15:07</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>2014/7/15 0:00:00</t>
+  </si>
+  <si>
+    <t>T3-A09-05-03,T3-A09-05-02,T3-A03-05-03,T3-A09-05-01,T3-A05-05-04,T3-A03-05-02,T3-A03-05-01</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>CP14071500003</t>
+  </si>
+  <si>
+    <t>2014/7/15 8:21:29</t>
+  </si>
+  <si>
+    <t>2014/7/15 8:26:00</t>
+  </si>
+  <si>
+    <t>T3-A03-05-04,T3-A01-05-01,T3-A01-05-02,T3-A01-05-03,T3-A09-05-04,T3-A07-05-01,T3-A07-05-02,T3-A07-05-03,T3-A07-05-04,T3-A05-05-01,T3-A05-05-02,T3-A05-05-03</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>CP14071500004</t>
+  </si>
+  <si>
+    <t>2014/7/15 9:44:19</t>
+  </si>
+  <si>
+    <t>2014/7/15 9:48:35</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>CP14071500005</t>
+  </si>
+  <si>
+    <t>2014/7/15 13:43:50</t>
+  </si>
+  <si>
+    <t>2014/7/15 13:46:51</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>CP14071500006</t>
+  </si>
+  <si>
+    <t>2014/7/15 16:03:33</t>
+  </si>
+  <si>
+    <t>2014/7/15 16:04:40</t>
+  </si>
+  <si>
+    <t>T1-E05-04-02</t>
   </si>
 </sst>
 </file>
@@ -491,7 +768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -560,6 +837,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -584,6 +862,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -595,12 +879,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,12 +890,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -659,7 +940,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -694,7 +975,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -909,15 +1190,15 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="3" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -933,13 +1214,13 @@
       <c r="E1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="9"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -955,8 +1236,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -971,8 +1252,8 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="34"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
@@ -985,8 +1266,8 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="35" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1001,8 +1282,8 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="35"/>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1015,8 +1296,8 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="35"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1029,8 +1310,8 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="35"/>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1043,8 +1324,8 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="35"/>
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
@@ -1057,8 +1338,8 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="33" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1073,8 +1354,8 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="36"/>
       <c r="B11" s="3"/>
       <c r="C11" s="7"/>
       <c r="D11" s="1"/>
@@ -1083,8 +1364,8 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="36"/>
       <c r="B12" s="3"/>
       <c r="C12" s="7"/>
       <c r="D12" s="1"/>
@@ -1093,8 +1374,8 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="36"/>
       <c r="B13" s="3"/>
       <c r="C13" s="7"/>
       <c r="D13" s="1"/>
@@ -1103,8 +1384,8 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="36"/>
       <c r="B14" s="3"/>
       <c r="C14" s="7"/>
       <c r="D14" s="1"/>
@@ -1113,8 +1394,8 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="36"/>
       <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
@@ -1127,8 +1408,8 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="36"/>
       <c r="B16" s="3"/>
       <c r="C16" s="7"/>
       <c r="D16" s="1"/>
@@ -1137,8 +1418,8 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" s="36"/>
       <c r="B17" s="3"/>
       <c r="C17" s="7"/>
       <c r="D17" s="1"/>
@@ -1147,8 +1428,8 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" s="36"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="D18" s="1"/>
@@ -1157,8 +1438,8 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19" s="36"/>
       <c r="B19" s="3"/>
       <c r="C19" s="7"/>
       <c r="D19" s="1"/>
@@ -1167,8 +1448,8 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20" s="36"/>
       <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
@@ -1181,8 +1462,8 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21" s="36"/>
       <c r="B21" s="4"/>
       <c r="C21" s="7"/>
       <c r="D21" s="1"/>
@@ -1191,8 +1472,8 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A22" s="34"/>
       <c r="B22" s="4"/>
       <c r="C22" s="7"/>
       <c r="D22" s="1"/>
@@ -1201,7 +1482,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="10"/>
       <c r="B23" s="4"/>
       <c r="C23" s="7"/>
@@ -1211,8 +1492,8 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A24" s="33" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1227,8 +1508,8 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A25" s="36"/>
       <c r="B25" s="3" t="s">
         <v>15</v>
       </c>
@@ -1241,8 +1522,8 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A26" s="34"/>
       <c r="B26" s="3" t="s">
         <v>16</v>
       </c>
@@ -1255,8 +1536,8 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1271,8 +1552,8 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A28" s="30"/>
       <c r="B28" s="4" t="s">
         <v>19</v>
       </c>
@@ -1285,7 +1566,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1313,21 +1594,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="26" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" style="27" customWidth="1"/>
-    <col min="4" max="4" width="52.77734375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="35.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16.375" style="26" customWidth="1"/>
+    <col min="3" max="3" width="22.125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="52.75" style="12" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="8" customWidth="1"/>
+    <col min="6" max="6" width="35.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1344,11 +1625,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+    <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.15">
+      <c r="A2" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="40" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1359,9 +1640,9 @@
       </c>
       <c r="E2" s="18"/>
     </row>
-    <row r="3" spans="1:5" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="38"/>
+    <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.15">
+      <c r="A3" s="42"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="13" t="s">
         <v>54</v>
       </c>
@@ -1370,9 +1651,9 @@
       </c>
       <c r="E3" s="18"/>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39" t="s">
+    <row r="4" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A4" s="42"/>
+      <c r="B4" s="42" t="s">
         <v>57</v>
       </c>
       <c r="C4" s="21" t="s">
@@ -1385,9 +1666,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
+    <row r="5" spans="1:5" ht="24" x14ac:dyDescent="0.15">
+      <c r="A5" s="42"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="22" t="s">
         <v>59</v>
       </c>
@@ -1396,8 +1677,8 @@
       </c>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:5" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
+    <row r="6" spans="1:5" ht="24" x14ac:dyDescent="0.15">
+      <c r="A6" s="42"/>
       <c r="B6" s="23" t="s">
         <v>31</v>
       </c>
@@ -1409,9 +1690,9 @@
       </c>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:5" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39" t="s">
+    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.15">
+      <c r="A7" s="42"/>
+      <c r="B7" s="42" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="22" t="s">
@@ -1422,9 +1703,9 @@
       </c>
       <c r="E7" s="18"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="42"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="13" t="s">
         <v>56</v>
       </c>
@@ -1433,8 +1714,8 @@
       </c>
       <c r="E8" s="18"/>
     </row>
-    <row r="9" spans="1:5" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="42"/>
       <c r="B9" s="20" t="s">
         <v>17</v>
       </c>
@@ -1446,18 +1727,18 @@
       </c>
       <c r="E9" s="18"/>
     </row>
-    <row r="10" spans="1:5" ht="2.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="24"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
       <c r="D10" s="15"/>
       <c r="E10" s="18"/>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+    <row r="11" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A11" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="39" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="13" t="s">
@@ -1468,18 +1749,18 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="13" t="s">
         <v>50</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="18"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="39"/>
+      <c r="B13" s="39" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="13" t="s">
@@ -1488,18 +1769,18 @@
       <c r="D13" s="15"/>
       <c r="E13" s="18"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="39"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="13" t="s">
         <v>80</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="18"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="39"/>
+      <c r="B15" s="39" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="13" t="s">
@@ -1508,17 +1789,17 @@
       <c r="D15" s="15"/>
       <c r="E15" s="18"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="39"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="18"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="39" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1530,8 +1811,8 @@
       <c r="D17" s="15"/>
       <c r="E17" s="18"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="39"/>
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1543,8 +1824,8 @@
       </c>
       <c r="E18" s="18"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="39"/>
       <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
@@ -1554,73 +1835,73 @@
       <c r="D19" s="15"/>
       <c r="E19" s="18"/>
     </row>
-    <row r="20" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
+    <row r="20" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="39" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="37" t="s">
         <v>48</v>
       </c>
       <c r="E20" s="18"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="41"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="18"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A22" s="39"/>
+      <c r="B22" s="39"/>
       <c r="C22" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="41"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36" t="s">
+    <row r="23" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="39"/>
+      <c r="B23" s="39" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="41" t="s">
+      <c r="D23" s="37" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="18"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" s="39"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="41"/>
+      <c r="D24" s="37"/>
       <c r="E24" s="18"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" s="39"/>
+      <c r="B25" s="39"/>
       <c r="C25" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="41"/>
+      <c r="D25" s="37"/>
       <c r="E25" s="18"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
-      <c r="B26" s="40" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" s="39"/>
+      <c r="B26" s="38" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="25" t="s">
@@ -1629,18 +1910,18 @@
       <c r="D26" s="15"/>
       <c r="E26" s="18"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
-      <c r="B27" s="40"/>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" s="39"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="25" t="s">
         <v>75</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="18"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
-      <c r="B28" s="40"/>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A28" s="39"/>
+      <c r="B28" s="38"/>
       <c r="C28" s="25" t="s">
         <v>30</v>
       </c>
@@ -1649,11 +1930,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="A11:A16"/>
     <mergeCell ref="B2:B3"/>
@@ -1662,6 +1938,11 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="B20:B22"/>
   </mergeCells>
@@ -1673,23 +1954,991 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>97</v>
+      </c>
+      <c r="R1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S1" t="s">
+        <v>99</v>
+      </c>
+      <c r="T1" t="s">
+        <v>100</v>
+      </c>
+      <c r="U1" t="s">
+        <v>101</v>
+      </c>
+      <c r="V1" t="s">
+        <v>102</v>
+      </c>
+      <c r="W1" t="s">
+        <v>103</v>
+      </c>
+      <c r="X1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A2" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="O2" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q2" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="R2" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="T2" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="U2" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="V2" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="W2" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="X2" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y2" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z2" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA2" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB2" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A3" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="M3" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="N3" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="O3" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="P3" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q3" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="R3" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="S3" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="T3" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="U3" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="V3" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="W3" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="X3" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y3" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z3" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA3" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB3" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A4" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="M4" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="N4" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="O4" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="P4" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q4" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="R4" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="S4" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="T4" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="U4" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="V4" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="W4" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="X4" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y4" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z4" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA4" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB4" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A5" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q5" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="R5" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="S5" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="T5" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="U5" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="V5" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="W5" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="X5" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y5" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z5" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA5" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB5" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A6" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="N6" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="O6" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="P6" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q6" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="R6" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="S6" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="T6" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="U6" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="V6" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="W6" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="X6" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y6" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z6" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA6" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB6" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A7" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="O7" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="P7" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q7" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="R7" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="S7" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="T7" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="U7" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="V7" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="W7" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="X7" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y7" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z7" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA7" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB7" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A8" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="L8" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="M8" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="N8" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="O8" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="P8" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q8" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="R8" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="S8" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="T8" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="U8" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="V8" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="W8" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="X8" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y8" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z8" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA8" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB8" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A9" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="J9" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="M9" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="N9" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="O9" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="P9" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q9" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="R9" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="S9" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="T9" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="U9" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="V9" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="W9" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="X9" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y9" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z9" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA9" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB9" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A10" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="L10" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="M10" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="N10" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="O10" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="P10" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q10" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="R10" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="S10" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="T10" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="U10" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="V10" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="W10" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="X10" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y10" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z10" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA10" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB10" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="A11" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="L11" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="M11" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="N11" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="O11" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="P11" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q11" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="R11" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="S11" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="T11" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="U11" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="V11" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="W11" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="X11" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y11" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z11" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA11" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB11" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>79</v>
       </c>

</xml_diff>